<commit_message>
Improved writing to file
</commit_message>
<xml_diff>
--- a/results/current-results.xlsx
+++ b/results/current-results.xlsx
@@ -24,43 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="468">
-  <si>
-    <t>ids_ 1</t>
-  </si>
-  <si>
-    <t>ids_ 2</t>
-  </si>
-  <si>
-    <t>ids_ 3</t>
-  </si>
-  <si>
-    <t>ids_ 4</t>
-  </si>
-  <si>
-    <t>ids_ 5</t>
-  </si>
-  <si>
-    <t>ids_ 6</t>
-  </si>
-  <si>
-    <t>ids_ 7</t>
-  </si>
-  <si>
-    <t>ids_ 8</t>
-  </si>
-  <si>
-    <t>ids_ 9</t>
-  </si>
-  <si>
-    <t>ids_10</t>
-  </si>
-  <si>
-    <t>ids_11</t>
-  </si>
-  <si>
-    <t>ids_12</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="468">
   <si>
     <t>ids_13</t>
   </si>
@@ -1428,6 +1392,42 @@
   </si>
   <si>
     <t>baselineSNRLeft_36</t>
+  </si>
+  <si>
+    <t>faceAmplitudeRight</t>
+  </si>
+  <si>
+    <t>baselineAmplitudeRight</t>
+  </si>
+  <si>
+    <t>faceAmplitudeLeft</t>
+  </si>
+  <si>
+    <t>baselineAmplitudeLeft</t>
+  </si>
+  <si>
+    <t>faceSNRRight</t>
+  </si>
+  <si>
+    <t>baselineSNRRight</t>
+  </si>
+  <si>
+    <t>faceSNRLeft</t>
+  </si>
+  <si>
+    <t>baselineSNRLeft</t>
+  </si>
+  <si>
+    <t>ids</t>
+  </si>
+  <si>
+    <t>aq</t>
+  </si>
+  <si>
+    <t>eq</t>
+  </si>
+  <si>
+    <t>sq</t>
   </si>
 </sst>
 </file>
@@ -1779,1420 +1779,1408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PP2"/>
+  <dimension ref="A1:PP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="MO1" workbookViewId="0">
-      <selection activeCell="MW1" sqref="MW1:PP2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:432" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="B1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1" t="s">
+        <v>467</v>
+      </c>
+      <c r="E1" t="s">
+        <v>456</v>
+      </c>
+      <c r="F1" t="s">
+        <v>457</v>
+      </c>
+      <c r="G1" t="s">
+        <v>458</v>
+      </c>
+      <c r="H1" t="s">
+        <v>459</v>
+      </c>
+      <c r="I1" t="s">
+        <v>460</v>
+      </c>
+      <c r="J1" t="s">
+        <v>461</v>
+      </c>
+      <c r="K1" t="s">
+        <v>462</v>
+      </c>
+      <c r="L1" t="s">
+        <v>463</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="O1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="P1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AI1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AJ1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AK1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AL1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AM1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AN1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AO1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AP1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AQ1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AR1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AS1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AT1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AU1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AV1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AW1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AX1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AY1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AZ1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BA1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BB1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BC1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BD1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BE1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BF1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BG1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BH1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BI1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BJ1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BK1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BL1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BM1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BN1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BO1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BP1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BQ1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BR1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BS1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BT1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BU1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BV1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BW1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BX1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BY1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BZ1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="CA1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="CB1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="CC1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="CD1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CE1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CF1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CG1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CH1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CI1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CJ1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CK1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CL1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CM1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CN1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CO1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CP1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CQ1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CR1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CS1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CT1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CU1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CV1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CW1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CX1" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CY1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CZ1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="DA1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="DB1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="DC1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="DD1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="DE1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DF1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DG1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DH1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DI1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DJ1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DK1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DL1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DM1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DN1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DO1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DP1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DQ1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DR1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DS1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DT1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DU1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DV1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DW1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DX1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DY1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DZ1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="EA1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="EB1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="EC1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="ED1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="EE1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="EF1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="EG1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="EH1" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="EI1" t="s">
         <v>126</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="EJ1" t="s">
         <v>127</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="EK1" t="s">
         <v>128</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EL1" t="s">
         <v>129</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EM1" t="s">
         <v>130</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EN1" t="s">
         <v>131</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="EO1" t="s">
         <v>132</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EP1" t="s">
         <v>133</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EQ1" t="s">
         <v>134</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="ER1" t="s">
         <v>135</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="ES1" t="s">
         <v>136</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="ET1" t="s">
         <v>137</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EU1" t="s">
         <v>138</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EV1" t="s">
         <v>139</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EW1" t="s">
         <v>140</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EX1" t="s">
         <v>141</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EY1" t="s">
         <v>142</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EZ1" t="s">
         <v>143</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="FA1" t="s">
         <v>144</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="FB1" t="s">
         <v>145</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="FC1" t="s">
         <v>146</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="FD1" t="s">
         <v>147</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="FE1" t="s">
         <v>148</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="FF1" t="s">
         <v>149</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="FG1" t="s">
         <v>150</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="FH1" t="s">
         <v>151</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="FI1" t="s">
         <v>152</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="FJ1" t="s">
         <v>153</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="FK1" t="s">
         <v>154</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FL1" t="s">
         <v>155</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FM1" t="s">
         <v>156</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="FN1" t="s">
         <v>157</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="FO1" t="s">
         <v>158</v>
       </c>
-      <c r="FD1" t="s">
+      <c r="FP1" t="s">
         <v>159</v>
       </c>
-      <c r="FE1" t="s">
+      <c r="FQ1" t="s">
         <v>160</v>
       </c>
-      <c r="FF1" t="s">
+      <c r="FR1" t="s">
         <v>161</v>
       </c>
-      <c r="FG1" t="s">
+      <c r="FS1" t="s">
         <v>162</v>
       </c>
-      <c r="FH1" t="s">
+      <c r="FT1" t="s">
         <v>163</v>
       </c>
-      <c r="FI1" t="s">
+      <c r="FU1" t="s">
         <v>164</v>
       </c>
-      <c r="FJ1" t="s">
+      <c r="FV1" t="s">
         <v>165</v>
       </c>
-      <c r="FK1" t="s">
+      <c r="FW1" t="s">
         <v>166</v>
       </c>
-      <c r="FL1" t="s">
+      <c r="FX1" t="s">
         <v>167</v>
       </c>
-      <c r="FM1" t="s">
+      <c r="FY1" t="s">
         <v>168</v>
       </c>
-      <c r="FN1" t="s">
+      <c r="FZ1" t="s">
         <v>169</v>
       </c>
-      <c r="FO1" t="s">
+      <c r="GA1" t="s">
         <v>170</v>
       </c>
-      <c r="FP1" t="s">
+      <c r="GB1" t="s">
         <v>171</v>
       </c>
-      <c r="FQ1" t="s">
+      <c r="GC1" t="s">
         <v>172</v>
       </c>
-      <c r="FR1" t="s">
+      <c r="GD1" t="s">
         <v>173</v>
       </c>
-      <c r="FS1" t="s">
+      <c r="GE1" t="s">
         <v>174</v>
       </c>
-      <c r="FT1" t="s">
+      <c r="GF1" t="s">
         <v>175</v>
       </c>
-      <c r="FU1" t="s">
+      <c r="GG1" t="s">
         <v>176</v>
       </c>
-      <c r="FV1" t="s">
+      <c r="GH1" t="s">
         <v>177</v>
       </c>
-      <c r="FW1" t="s">
+      <c r="GI1" t="s">
         <v>178</v>
       </c>
-      <c r="FX1" t="s">
+      <c r="GJ1" t="s">
         <v>179</v>
       </c>
-      <c r="FY1" t="s">
+      <c r="GK1" t="s">
         <v>180</v>
       </c>
-      <c r="FZ1" t="s">
+      <c r="GL1" t="s">
         <v>181</v>
       </c>
-      <c r="GA1" t="s">
+      <c r="GM1" t="s">
         <v>182</v>
       </c>
-      <c r="GB1" t="s">
+      <c r="GN1" t="s">
         <v>183</v>
       </c>
-      <c r="GC1" t="s">
+      <c r="GO1" t="s">
         <v>184</v>
       </c>
-      <c r="GD1" t="s">
+      <c r="GP1" t="s">
         <v>185</v>
       </c>
-      <c r="GE1" t="s">
+      <c r="GQ1" t="s">
         <v>186</v>
       </c>
-      <c r="GF1" t="s">
+      <c r="GR1" t="s">
         <v>187</v>
       </c>
-      <c r="GG1" t="s">
+      <c r="GS1" t="s">
         <v>188</v>
       </c>
-      <c r="GH1" t="s">
+      <c r="GT1" t="s">
         <v>189</v>
       </c>
-      <c r="GI1" t="s">
+      <c r="GU1" t="s">
         <v>190</v>
       </c>
-      <c r="GJ1" t="s">
+      <c r="GV1" t="s">
         <v>191</v>
       </c>
-      <c r="GK1" t="s">
+      <c r="GW1" t="s">
         <v>192</v>
       </c>
-      <c r="GL1" t="s">
+      <c r="GX1" t="s">
         <v>193</v>
       </c>
-      <c r="GM1" t="s">
+      <c r="GY1" t="s">
         <v>194</v>
       </c>
-      <c r="GN1" t="s">
+      <c r="GZ1" t="s">
         <v>195</v>
       </c>
-      <c r="GO1" t="s">
+      <c r="HA1" t="s">
         <v>196</v>
       </c>
-      <c r="GP1" t="s">
+      <c r="HB1" t="s">
         <v>197</v>
       </c>
-      <c r="GQ1" t="s">
+      <c r="HC1" t="s">
         <v>198</v>
       </c>
-      <c r="GR1" t="s">
+      <c r="HD1" t="s">
         <v>199</v>
       </c>
-      <c r="GS1" t="s">
+      <c r="HE1" t="s">
         <v>200</v>
       </c>
-      <c r="GT1" t="s">
+      <c r="HF1" t="s">
         <v>201</v>
       </c>
-      <c r="GU1" t="s">
+      <c r="HG1" t="s">
         <v>202</v>
       </c>
-      <c r="GV1" t="s">
+      <c r="HH1" t="s">
         <v>203</v>
       </c>
-      <c r="GW1" t="s">
+      <c r="HI1" t="s">
         <v>204</v>
       </c>
-      <c r="GX1" t="s">
+      <c r="HJ1" t="s">
         <v>205</v>
       </c>
-      <c r="GY1" t="s">
+      <c r="HK1" t="s">
         <v>206</v>
       </c>
-      <c r="GZ1" t="s">
+      <c r="HL1" t="s">
         <v>207</v>
       </c>
-      <c r="HA1" t="s">
+      <c r="HM1" t="s">
         <v>208</v>
       </c>
-      <c r="HB1" t="s">
+      <c r="HN1" t="s">
         <v>209</v>
       </c>
-      <c r="HC1" t="s">
+      <c r="HO1" t="s">
         <v>210</v>
       </c>
-      <c r="HD1" t="s">
+      <c r="HP1" t="s">
         <v>211</v>
       </c>
-      <c r="HE1" t="s">
+      <c r="HQ1" t="s">
         <v>212</v>
       </c>
-      <c r="HF1" t="s">
+      <c r="HR1" t="s">
         <v>213</v>
       </c>
-      <c r="HG1" t="s">
+      <c r="HS1" t="s">
         <v>214</v>
       </c>
-      <c r="HH1" t="s">
+      <c r="HT1" t="s">
         <v>215</v>
       </c>
-      <c r="HI1" t="s">
+      <c r="HU1" t="s">
         <v>216</v>
       </c>
-      <c r="HJ1" t="s">
+      <c r="HV1" t="s">
         <v>217</v>
       </c>
-      <c r="HK1" t="s">
+      <c r="HW1" t="s">
         <v>218</v>
       </c>
-      <c r="HL1" t="s">
+      <c r="HX1" t="s">
         <v>219</v>
       </c>
-      <c r="HM1" t="s">
+      <c r="HY1" t="s">
         <v>220</v>
       </c>
-      <c r="HN1" t="s">
+      <c r="HZ1" t="s">
         <v>221</v>
       </c>
-      <c r="HO1" t="s">
+      <c r="IA1" t="s">
         <v>222</v>
       </c>
-      <c r="HP1" t="s">
+      <c r="IB1" t="s">
         <v>223</v>
       </c>
-      <c r="HQ1" t="s">
+      <c r="IC1" t="s">
         <v>224</v>
       </c>
-      <c r="HR1" t="s">
+      <c r="ID1" t="s">
         <v>225</v>
       </c>
-      <c r="HS1" t="s">
+      <c r="IE1" t="s">
         <v>226</v>
       </c>
-      <c r="HT1" t="s">
+      <c r="IF1" t="s">
         <v>227</v>
       </c>
-      <c r="HU1" t="s">
+      <c r="IG1" t="s">
         <v>228</v>
       </c>
-      <c r="HV1" t="s">
+      <c r="IH1" t="s">
         <v>229</v>
       </c>
-      <c r="HW1" t="s">
+      <c r="II1" t="s">
         <v>230</v>
       </c>
-      <c r="HX1" t="s">
+      <c r="IJ1" t="s">
         <v>231</v>
       </c>
-      <c r="HY1" t="s">
+      <c r="IK1" t="s">
         <v>232</v>
       </c>
-      <c r="HZ1" t="s">
+      <c r="IL1" t="s">
         <v>233</v>
       </c>
-      <c r="IA1" t="s">
+      <c r="IM1" t="s">
         <v>234</v>
       </c>
-      <c r="IB1" t="s">
+      <c r="IN1" t="s">
         <v>235</v>
       </c>
-      <c r="IC1" t="s">
+      <c r="IO1" t="s">
         <v>236</v>
       </c>
-      <c r="ID1" t="s">
+      <c r="IP1" t="s">
         <v>237</v>
       </c>
-      <c r="IE1" t="s">
+      <c r="IQ1" t="s">
         <v>238</v>
       </c>
-      <c r="IF1" t="s">
+      <c r="IR1" t="s">
         <v>239</v>
       </c>
-      <c r="IG1" t="s">
+      <c r="IS1" t="s">
         <v>240</v>
       </c>
-      <c r="IH1" t="s">
+      <c r="IT1" t="s">
         <v>241</v>
       </c>
-      <c r="II1" t="s">
+      <c r="IU1" t="s">
         <v>242</v>
       </c>
-      <c r="IJ1" t="s">
+      <c r="IV1" t="s">
         <v>243</v>
       </c>
-      <c r="IK1" t="s">
+      <c r="IW1" t="s">
         <v>244</v>
       </c>
-      <c r="IL1" t="s">
+      <c r="IX1" t="s">
         <v>245</v>
       </c>
-      <c r="IM1" t="s">
+      <c r="IY1" t="s">
         <v>246</v>
       </c>
-      <c r="IN1" t="s">
+      <c r="IZ1" t="s">
         <v>247</v>
       </c>
-      <c r="IO1" t="s">
+      <c r="JA1" t="s">
         <v>248</v>
       </c>
-      <c r="IP1" t="s">
+      <c r="JB1" t="s">
         <v>249</v>
       </c>
-      <c r="IQ1" t="s">
+      <c r="JC1" t="s">
         <v>250</v>
       </c>
-      <c r="IR1" t="s">
+      <c r="JD1" t="s">
         <v>251</v>
       </c>
-      <c r="IS1" t="s">
+      <c r="JE1" t="s">
         <v>252</v>
       </c>
-      <c r="IT1" t="s">
+      <c r="JF1" t="s">
         <v>253</v>
       </c>
-      <c r="IU1" t="s">
+      <c r="JG1" t="s">
         <v>254</v>
       </c>
-      <c r="IV1" t="s">
+      <c r="JH1" t="s">
         <v>255</v>
       </c>
-      <c r="IW1" t="s">
+      <c r="JI1" t="s">
         <v>256</v>
       </c>
-      <c r="IX1" t="s">
+      <c r="JJ1" t="s">
         <v>257</v>
       </c>
-      <c r="IY1" t="s">
+      <c r="JK1" t="s">
         <v>258</v>
       </c>
-      <c r="IZ1" t="s">
+      <c r="JL1" t="s">
         <v>259</v>
       </c>
-      <c r="JA1" t="s">
+      <c r="JM1" t="s">
         <v>260</v>
       </c>
-      <c r="JB1" t="s">
+      <c r="JN1" t="s">
         <v>261</v>
       </c>
-      <c r="JC1" t="s">
+      <c r="JO1" t="s">
         <v>262</v>
       </c>
-      <c r="JD1" t="s">
+      <c r="JP1" t="s">
         <v>263</v>
       </c>
-      <c r="JE1" t="s">
+      <c r="JQ1" t="s">
         <v>264</v>
       </c>
-      <c r="JF1" t="s">
+      <c r="JR1" t="s">
         <v>265</v>
       </c>
-      <c r="JG1" t="s">
+      <c r="JS1" t="s">
         <v>266</v>
       </c>
-      <c r="JH1" t="s">
+      <c r="JT1" t="s">
         <v>267</v>
       </c>
-      <c r="JI1" t="s">
+      <c r="JU1" t="s">
         <v>268</v>
       </c>
-      <c r="JJ1" t="s">
+      <c r="JV1" t="s">
         <v>269</v>
       </c>
-      <c r="JK1" t="s">
+      <c r="JW1" t="s">
         <v>270</v>
       </c>
-      <c r="JL1" t="s">
+      <c r="JX1" t="s">
         <v>271</v>
       </c>
-      <c r="JM1" t="s">
+      <c r="JY1" t="s">
         <v>272</v>
       </c>
-      <c r="JN1" t="s">
+      <c r="JZ1" t="s">
         <v>273</v>
       </c>
-      <c r="JO1" t="s">
+      <c r="KA1" t="s">
         <v>274</v>
       </c>
-      <c r="JP1" t="s">
+      <c r="KB1" t="s">
         <v>275</v>
       </c>
-      <c r="JQ1" t="s">
+      <c r="KC1" t="s">
         <v>276</v>
       </c>
-      <c r="JR1" t="s">
+      <c r="KD1" t="s">
         <v>277</v>
       </c>
-      <c r="JS1" t="s">
+      <c r="KE1" t="s">
         <v>278</v>
       </c>
-      <c r="JT1" t="s">
+      <c r="KF1" t="s">
         <v>279</v>
       </c>
-      <c r="JU1" t="s">
+      <c r="KG1" t="s">
         <v>280</v>
       </c>
-      <c r="JV1" t="s">
+      <c r="KH1" t="s">
         <v>281</v>
       </c>
-      <c r="JW1" t="s">
+      <c r="KI1" t="s">
         <v>282</v>
       </c>
-      <c r="JX1" t="s">
+      <c r="KJ1" t="s">
         <v>283</v>
       </c>
-      <c r="JY1" t="s">
+      <c r="KK1" t="s">
         <v>284</v>
       </c>
-      <c r="JZ1" t="s">
+      <c r="KL1" t="s">
         <v>285</v>
       </c>
-      <c r="KA1" t="s">
+      <c r="KM1" t="s">
         <v>286</v>
       </c>
-      <c r="KB1" t="s">
+      <c r="KN1" t="s">
         <v>287</v>
       </c>
-      <c r="KC1" t="s">
+      <c r="KO1" t="s">
         <v>288</v>
       </c>
-      <c r="KD1" t="s">
+      <c r="KP1" t="s">
         <v>289</v>
       </c>
-      <c r="KE1" t="s">
+      <c r="KQ1" t="s">
         <v>290</v>
       </c>
-      <c r="KF1" t="s">
+      <c r="KR1" t="s">
         <v>291</v>
       </c>
-      <c r="KG1" t="s">
+      <c r="KS1" t="s">
         <v>292</v>
       </c>
-      <c r="KH1" t="s">
+      <c r="KT1" t="s">
         <v>293</v>
       </c>
-      <c r="KI1" t="s">
+      <c r="KU1" t="s">
         <v>294</v>
       </c>
-      <c r="KJ1" t="s">
+      <c r="KV1" t="s">
         <v>295</v>
       </c>
-      <c r="KK1" t="s">
+      <c r="KW1" t="s">
         <v>296</v>
       </c>
-      <c r="KL1" t="s">
+      <c r="KX1" t="s">
         <v>297</v>
       </c>
-      <c r="KM1" t="s">
+      <c r="KY1" t="s">
         <v>298</v>
       </c>
-      <c r="KN1" t="s">
+      <c r="KZ1" t="s">
         <v>299</v>
       </c>
-      <c r="KO1" t="s">
+      <c r="LA1" t="s">
         <v>300</v>
       </c>
-      <c r="KP1" t="s">
+      <c r="LB1" t="s">
         <v>301</v>
       </c>
-      <c r="KQ1" t="s">
+      <c r="LC1" t="s">
         <v>302</v>
       </c>
-      <c r="KR1" t="s">
+      <c r="LD1" t="s">
         <v>303</v>
       </c>
-      <c r="KS1" t="s">
+      <c r="LE1" t="s">
         <v>304</v>
       </c>
-      <c r="KT1" t="s">
+      <c r="LF1" t="s">
         <v>305</v>
       </c>
-      <c r="KU1" t="s">
+      <c r="LG1" t="s">
         <v>306</v>
       </c>
-      <c r="KV1" t="s">
+      <c r="LH1" t="s">
         <v>307</v>
       </c>
-      <c r="KW1" t="s">
+      <c r="LI1" t="s">
         <v>308</v>
       </c>
-      <c r="KX1" t="s">
+      <c r="LJ1" t="s">
         <v>309</v>
       </c>
-      <c r="KY1" t="s">
+      <c r="LK1" t="s">
         <v>310</v>
       </c>
-      <c r="KZ1" t="s">
+      <c r="LL1" t="s">
         <v>311</v>
       </c>
-      <c r="LA1" t="s">
+      <c r="LM1" t="s">
         <v>312</v>
       </c>
-      <c r="LB1" t="s">
+      <c r="LN1" t="s">
         <v>313</v>
       </c>
-      <c r="LC1" t="s">
+      <c r="LO1" t="s">
         <v>314</v>
       </c>
-      <c r="LD1" t="s">
+      <c r="LP1" t="s">
         <v>315</v>
       </c>
-      <c r="LE1" t="s">
+      <c r="LQ1" t="s">
         <v>316</v>
       </c>
-      <c r="LF1" t="s">
+      <c r="LR1" t="s">
         <v>317</v>
       </c>
-      <c r="LG1" t="s">
+      <c r="LS1" t="s">
         <v>318</v>
       </c>
-      <c r="LH1" t="s">
+      <c r="LT1" t="s">
         <v>319</v>
       </c>
-      <c r="LI1" t="s">
+      <c r="LU1" t="s">
         <v>320</v>
       </c>
-      <c r="LJ1" t="s">
+      <c r="LV1" t="s">
         <v>321</v>
       </c>
-      <c r="LK1" t="s">
+      <c r="LW1" t="s">
         <v>322</v>
       </c>
-      <c r="LL1" t="s">
+      <c r="LX1" t="s">
         <v>323</v>
       </c>
-      <c r="LM1" t="s">
+      <c r="LY1" t="s">
         <v>324</v>
       </c>
-      <c r="LN1" t="s">
+      <c r="LZ1" t="s">
         <v>325</v>
       </c>
-      <c r="LO1" t="s">
+      <c r="MA1" t="s">
         <v>326</v>
       </c>
-      <c r="LP1" t="s">
+      <c r="MB1" t="s">
         <v>327</v>
       </c>
-      <c r="LQ1" t="s">
+      <c r="MC1" t="s">
         <v>328</v>
       </c>
-      <c r="LR1" t="s">
+      <c r="MD1" t="s">
         <v>329</v>
       </c>
-      <c r="LS1" t="s">
+      <c r="ME1" t="s">
         <v>330</v>
       </c>
-      <c r="LT1" t="s">
+      <c r="MF1" t="s">
         <v>331</v>
       </c>
-      <c r="LU1" t="s">
+      <c r="MG1" t="s">
         <v>332</v>
       </c>
-      <c r="LV1" t="s">
+      <c r="MH1" t="s">
         <v>333</v>
       </c>
-      <c r="LW1" t="s">
+      <c r="MI1" t="s">
         <v>334</v>
       </c>
-      <c r="LX1" t="s">
+      <c r="MJ1" t="s">
         <v>335</v>
       </c>
-      <c r="LY1" t="s">
+      <c r="MK1" t="s">
         <v>336</v>
       </c>
-      <c r="LZ1" t="s">
+      <c r="ML1" t="s">
         <v>337</v>
       </c>
-      <c r="MA1" t="s">
+      <c r="MM1" t="s">
         <v>338</v>
       </c>
-      <c r="MB1" t="s">
+      <c r="MN1" t="s">
         <v>339</v>
       </c>
-      <c r="MC1" t="s">
+      <c r="MO1" t="s">
         <v>340</v>
       </c>
-      <c r="MD1" t="s">
+      <c r="MP1" t="s">
         <v>341</v>
       </c>
-      <c r="ME1" t="s">
+      <c r="MQ1" t="s">
         <v>342</v>
       </c>
-      <c r="MF1" t="s">
+      <c r="MR1" t="s">
         <v>343</v>
       </c>
-      <c r="MG1" t="s">
+      <c r="MS1" t="s">
         <v>344</v>
       </c>
-      <c r="MH1" t="s">
+      <c r="MT1" t="s">
         <v>345</v>
       </c>
-      <c r="MI1" t="s">
+      <c r="MU1" t="s">
         <v>346</v>
       </c>
-      <c r="MJ1" t="s">
+      <c r="MV1" t="s">
         <v>347</v>
       </c>
-      <c r="MK1" t="s">
-        <v>348</v>
-      </c>
-      <c r="ML1" t="s">
-        <v>349</v>
-      </c>
-      <c r="MM1" t="s">
-        <v>350</v>
-      </c>
-      <c r="MN1" t="s">
-        <v>351</v>
-      </c>
-      <c r="MO1" t="s">
-        <v>352</v>
-      </c>
-      <c r="MP1" t="s">
-        <v>353</v>
-      </c>
-      <c r="MQ1" t="s">
-        <v>354</v>
-      </c>
-      <c r="MR1" t="s">
-        <v>355</v>
-      </c>
-      <c r="MS1" t="s">
-        <v>356</v>
-      </c>
-      <c r="MT1" t="s">
-        <v>357</v>
-      </c>
-      <c r="MU1" t="s">
-        <v>358</v>
-      </c>
-      <c r="MV1" t="s">
-        <v>359</v>
-      </c>
       <c r="MW1" t="s">
+        <v>384</v>
+      </c>
+      <c r="MX1" t="s">
+        <v>385</v>
+      </c>
+      <c r="MY1" t="s">
+        <v>386</v>
+      </c>
+      <c r="MZ1" t="s">
+        <v>387</v>
+      </c>
+      <c r="NA1" t="s">
+        <v>388</v>
+      </c>
+      <c r="NB1" t="s">
+        <v>389</v>
+      </c>
+      <c r="NC1" t="s">
+        <v>390</v>
+      </c>
+      <c r="ND1" t="s">
+        <v>391</v>
+      </c>
+      <c r="NE1" t="s">
+        <v>392</v>
+      </c>
+      <c r="NF1" t="s">
+        <v>393</v>
+      </c>
+      <c r="NG1" t="s">
+        <v>394</v>
+      </c>
+      <c r="NH1" t="s">
+        <v>395</v>
+      </c>
+      <c r="NI1" t="s">
         <v>396</v>
       </c>
-      <c r="MX1" t="s">
+      <c r="NJ1" t="s">
         <v>397</v>
       </c>
-      <c r="MY1" t="s">
+      <c r="NK1" t="s">
         <v>398</v>
       </c>
-      <c r="MZ1" t="s">
+      <c r="NL1" t="s">
         <v>399</v>
       </c>
-      <c r="NA1" t="s">
+      <c r="NM1" t="s">
         <v>400</v>
       </c>
-      <c r="NB1" t="s">
+      <c r="NN1" t="s">
         <v>401</v>
       </c>
-      <c r="NC1" t="s">
+      <c r="NO1" t="s">
         <v>402</v>
       </c>
-      <c r="ND1" t="s">
+      <c r="NP1" t="s">
         <v>403</v>
       </c>
-      <c r="NE1" t="s">
+      <c r="NQ1" t="s">
         <v>404</v>
       </c>
-      <c r="NF1" t="s">
+      <c r="NR1" t="s">
         <v>405</v>
       </c>
-      <c r="NG1" t="s">
+      <c r="NS1" t="s">
         <v>406</v>
       </c>
-      <c r="NH1" t="s">
+      <c r="NT1" t="s">
         <v>407</v>
       </c>
-      <c r="NI1" t="s">
+      <c r="NU1" t="s">
         <v>408</v>
       </c>
-      <c r="NJ1" t="s">
+      <c r="NV1" t="s">
         <v>409</v>
       </c>
-      <c r="NK1" t="s">
+      <c r="NW1" t="s">
         <v>410</v>
       </c>
-      <c r="NL1" t="s">
+      <c r="NX1" t="s">
         <v>411</v>
       </c>
-      <c r="NM1" t="s">
+      <c r="NY1" t="s">
         <v>412</v>
       </c>
-      <c r="NN1" t="s">
+      <c r="NZ1" t="s">
         <v>413</v>
       </c>
-      <c r="NO1" t="s">
+      <c r="OA1" t="s">
         <v>414</v>
       </c>
-      <c r="NP1" t="s">
+      <c r="OB1" t="s">
         <v>415</v>
       </c>
-      <c r="NQ1" t="s">
+      <c r="OC1" t="s">
         <v>416</v>
       </c>
-      <c r="NR1" t="s">
+      <c r="OD1" t="s">
         <v>417</v>
       </c>
-      <c r="NS1" t="s">
+      <c r="OE1" t="s">
         <v>418</v>
       </c>
-      <c r="NT1" t="s">
+      <c r="OF1" t="s">
         <v>419</v>
       </c>
-      <c r="NU1" t="s">
+      <c r="OG1" t="s">
         <v>420</v>
       </c>
-      <c r="NV1" t="s">
+      <c r="OH1" t="s">
         <v>421</v>
       </c>
-      <c r="NW1" t="s">
+      <c r="OI1" t="s">
         <v>422</v>
       </c>
-      <c r="NX1" t="s">
+      <c r="OJ1" t="s">
         <v>423</v>
       </c>
-      <c r="NY1" t="s">
+      <c r="OK1" t="s">
         <v>424</v>
       </c>
-      <c r="NZ1" t="s">
+      <c r="OL1" t="s">
         <v>425</v>
       </c>
-      <c r="OA1" t="s">
+      <c r="OM1" t="s">
         <v>426</v>
       </c>
-      <c r="OB1" t="s">
+      <c r="ON1" t="s">
         <v>427</v>
       </c>
-      <c r="OC1" t="s">
+      <c r="OO1" t="s">
         <v>428</v>
       </c>
-      <c r="OD1" t="s">
+      <c r="OP1" t="s">
         <v>429</v>
       </c>
-      <c r="OE1" t="s">
+      <c r="OQ1" t="s">
         <v>430</v>
       </c>
-      <c r="OF1" t="s">
+      <c r="OR1" t="s">
         <v>431</v>
       </c>
-      <c r="OG1" t="s">
+      <c r="OS1" t="s">
         <v>432</v>
       </c>
-      <c r="OH1" t="s">
+      <c r="OT1" t="s">
         <v>433</v>
       </c>
-      <c r="OI1" t="s">
+      <c r="OU1" t="s">
         <v>434</v>
       </c>
-      <c r="OJ1" t="s">
+      <c r="OV1" t="s">
         <v>435</v>
       </c>
-      <c r="OK1" t="s">
+      <c r="OW1" t="s">
         <v>436</v>
       </c>
-      <c r="OL1" t="s">
+      <c r="OX1" t="s">
         <v>437</v>
       </c>
-      <c r="OM1" t="s">
+      <c r="OY1" t="s">
         <v>438</v>
       </c>
-      <c r="ON1" t="s">
+      <c r="OZ1" t="s">
         <v>439</v>
       </c>
-      <c r="OO1" t="s">
+      <c r="PA1" t="s">
         <v>440</v>
       </c>
-      <c r="OP1" t="s">
+      <c r="PB1" t="s">
         <v>441</v>
       </c>
-      <c r="OQ1" t="s">
+      <c r="PC1" t="s">
         <v>442</v>
       </c>
-      <c r="OR1" t="s">
+      <c r="PD1" t="s">
         <v>443</v>
       </c>
-      <c r="OS1" t="s">
+      <c r="PE1" t="s">
         <v>444</v>
       </c>
-      <c r="OT1" t="s">
+      <c r="PF1" t="s">
         <v>445</v>
       </c>
-      <c r="OU1" t="s">
+      <c r="PG1" t="s">
         <v>446</v>
       </c>
-      <c r="OV1" t="s">
+      <c r="PH1" t="s">
         <v>447</v>
       </c>
-      <c r="OW1" t="s">
+      <c r="PI1" t="s">
         <v>448</v>
       </c>
-      <c r="OX1" t="s">
+      <c r="PJ1" t="s">
         <v>449</v>
       </c>
-      <c r="OY1" t="s">
+      <c r="PK1" t="s">
         <v>450</v>
       </c>
-      <c r="OZ1" t="s">
+      <c r="PL1" t="s">
         <v>451</v>
       </c>
-      <c r="PA1" t="s">
+      <c r="PM1" t="s">
         <v>452</v>
       </c>
-      <c r="PB1" t="s">
+      <c r="PN1" t="s">
         <v>453</v>
       </c>
-      <c r="PC1" t="s">
+      <c r="PO1" t="s">
         <v>454</v>
       </c>
-      <c r="PD1" t="s">
+      <c r="PP1" t="s">
         <v>455</v>
-      </c>
-      <c r="PE1" t="s">
-        <v>456</v>
-      </c>
-      <c r="PF1" t="s">
-        <v>457</v>
-      </c>
-      <c r="PG1" t="s">
-        <v>458</v>
-      </c>
-      <c r="PH1" t="s">
-        <v>459</v>
-      </c>
-      <c r="PI1" t="s">
-        <v>460</v>
-      </c>
-      <c r="PJ1" t="s">
-        <v>461</v>
-      </c>
-      <c r="PK1" t="s">
-        <v>462</v>
-      </c>
-      <c r="PL1" t="s">
-        <v>463</v>
-      </c>
-      <c r="PM1" t="s">
-        <v>464</v>
-      </c>
-      <c r="PN1" t="s">
-        <v>465</v>
-      </c>
-      <c r="PO1" t="s">
-        <v>466</v>
-      </c>
-      <c r="PP1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:432" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
         <v>360</v>
       </c>
-      <c r="B2" t="s">
+      <c r="N2" t="s">
         <v>361</v>
       </c>
-      <c r="C2" t="s">
+      <c r="O2" t="s">
         <v>362</v>
       </c>
-      <c r="D2" t="s">
+      <c r="P2" t="s">
         <v>363</v>
       </c>
-      <c r="E2" t="s">
+      <c r="Q2" t="s">
         <v>364</v>
       </c>
-      <c r="F2" t="s">
+      <c r="R2" t="s">
         <v>365</v>
       </c>
-      <c r="G2" t="s">
+      <c r="S2" t="s">
         <v>366</v>
       </c>
-      <c r="H2" t="s">
+      <c r="T2" t="s">
         <v>367</v>
       </c>
-      <c r="I2" t="s">
+      <c r="U2" t="s">
         <v>368</v>
       </c>
-      <c r="J2" t="s">
+      <c r="V2" t="s">
         <v>369</v>
       </c>
-      <c r="K2" t="s">
+      <c r="W2" t="s">
         <v>370</v>
       </c>
-      <c r="L2" t="s">
+      <c r="X2" t="s">
         <v>371</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Y2" t="s">
         <v>372</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Z2" t="s">
         <v>373</v>
       </c>
-      <c r="O2" t="s">
+      <c r="AA2" t="s">
         <v>374</v>
       </c>
-      <c r="P2" t="s">
+      <c r="AB2" t="s">
         <v>375</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AC2" t="s">
         <v>376</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AD2" t="s">
         <v>377</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AE2" t="s">
         <v>378</v>
       </c>
-      <c r="T2" t="s">
+      <c r="AF2" t="s">
         <v>379</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AG2" t="s">
         <v>380</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AH2" t="s">
         <v>381</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AI2" t="s">
         <v>382</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AJ2" t="s">
         <v>383</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>384</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>385</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>386</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>387</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>388</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>389</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>390</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>391</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>392</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>393</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>394</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>395</v>
       </c>
       <c r="AK2">
         <v>32</v>
@@ -4218,6 +4206,1186 @@
         <v>2.1497725233622482</v>
       </c>
       <c r="PP2">
+        <v>7.4920642694560105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>87</v>
+      </c>
+      <c r="E3">
+        <v>1.347492576784342</v>
+      </c>
+      <c r="F3">
+        <v>1.8445682011570605</v>
+      </c>
+      <c r="G3">
+        <v>0.78152237286994874</v>
+      </c>
+      <c r="H3">
+        <v>0.89553803933079623</v>
+      </c>
+      <c r="I3">
+        <v>2.4185715986187168</v>
+      </c>
+      <c r="J3">
+        <v>14.937623340803187</v>
+      </c>
+      <c r="K3">
+        <v>1.3354452699664794</v>
+      </c>
+      <c r="L3">
+        <v>8.9417721297661839</v>
+      </c>
+    </row>
+    <row r="4" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>1.1578328427695495</v>
+      </c>
+      <c r="F4">
+        <v>0.19670776526812772</v>
+      </c>
+      <c r="G4">
+        <v>0.60893120790003441</v>
+      </c>
+      <c r="H4">
+        <v>0.15423666671021558</v>
+      </c>
+      <c r="I4">
+        <v>1.323052104056778</v>
+      </c>
+      <c r="J4">
+        <v>1.6796747682529429</v>
+      </c>
+      <c r="K4">
+        <v>1.4493123981262919</v>
+      </c>
+      <c r="L4">
+        <v>2.5959884182876278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>104</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>128</v>
+      </c>
+      <c r="E6">
+        <v>0.75644995964610828</v>
+      </c>
+      <c r="F6">
+        <v>0.62010218883460166</v>
+      </c>
+      <c r="G6">
+        <v>1.3595540556176686</v>
+      </c>
+      <c r="H6">
+        <v>0.28128687598400598</v>
+      </c>
+      <c r="I6">
+        <v>1.8111087145058071</v>
+      </c>
+      <c r="J6">
+        <v>3.4213983079832651</v>
+      </c>
+      <c r="K6">
+        <v>1.4380309268942366</v>
+      </c>
+      <c r="L6">
+        <v>0.82870890467587754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>43</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>55</v>
+      </c>
+      <c r="E8">
+        <v>1.0543207747612136</v>
+      </c>
+      <c r="F8">
+        <v>1.479321020626962</v>
+      </c>
+      <c r="G8">
+        <v>0.73780126617805364</v>
+      </c>
+      <c r="H8">
+        <v>0.48412545942977225</v>
+      </c>
+      <c r="I8">
+        <v>1.55693272373023</v>
+      </c>
+      <c r="J8">
+        <v>11.746210284587853</v>
+      </c>
+      <c r="K8">
+        <v>1.239421135968404</v>
+      </c>
+      <c r="L8">
+        <v>4.0471003087409416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="D9">
+        <v>61</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>55</v>
+      </c>
+      <c r="D10">
+        <v>49</v>
+      </c>
+      <c r="E10">
+        <v>0.85875493905558864</v>
+      </c>
+      <c r="F10">
+        <v>0.17474741231064733</v>
+      </c>
+      <c r="G10">
+        <v>0.78691628171220918</v>
+      </c>
+      <c r="H10">
+        <v>0.49787353326798689</v>
+      </c>
+      <c r="I10">
+        <v>2.9076215013301625</v>
+      </c>
+      <c r="J10">
+        <v>2.7781622713728886</v>
+      </c>
+      <c r="K10">
+        <v>2.691034185036937</v>
+      </c>
+      <c r="L10">
+        <v>6.5475185824165569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>357</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>1.5428406744858454</v>
+      </c>
+      <c r="F11">
+        <v>2.2404850727410883</v>
+      </c>
+      <c r="G11">
+        <v>0.78727189894754057</v>
+      </c>
+      <c r="H11">
+        <v>0.28440402162053535</v>
+      </c>
+      <c r="I11">
+        <v>1.4621268191926056</v>
+      </c>
+      <c r="J11">
+        <v>7.1553487857147609</v>
+      </c>
+      <c r="K11">
+        <v>1.1390281524004433</v>
+      </c>
+      <c r="L11">
+        <v>1.4053678990778975</v>
+      </c>
+    </row>
+    <row r="12" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>358</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>0.77205311883192773</v>
+      </c>
+      <c r="F12">
+        <v>0.26864891089545762</v>
+      </c>
+      <c r="G12">
+        <v>0.52755160635362497</v>
+      </c>
+      <c r="H12">
+        <v>0.30568485900978792</v>
+      </c>
+      <c r="I12">
+        <v>2.3524335352791392</v>
+      </c>
+      <c r="J12">
+        <v>3.5036514661854796</v>
+      </c>
+      <c r="K12">
+        <v>1.2180583451008715</v>
+      </c>
+      <c r="L12">
+        <v>3.9514714348707023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>359</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>34</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>360</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>65</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B15">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>46</v>
+      </c>
+      <c r="D15">
+        <v>68</v>
+      </c>
+      <c r="E15">
+        <v>0.54932410435206969</v>
+      </c>
+      <c r="F15">
+        <v>0.55635001685181562</v>
+      </c>
+      <c r="G15">
+        <v>0.3604700397741647</v>
+      </c>
+      <c r="H15">
+        <v>0.51541915399296478</v>
+      </c>
+      <c r="I15">
+        <v>1.3836355829093936</v>
+      </c>
+      <c r="J15">
+        <v>4.9165853843329792</v>
+      </c>
+      <c r="K15">
+        <v>1.1171613085339864</v>
+      </c>
+      <c r="L15">
+        <v>4.8991800781321571</v>
+      </c>
+    </row>
+    <row r="16" spans="1:432" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>44</v>
+      </c>
+      <c r="D16">
+        <v>73</v>
+      </c>
+      <c r="E16">
+        <v>1.2382739403709864</v>
+      </c>
+      <c r="F16">
+        <v>0.9407468890980909</v>
+      </c>
+      <c r="G16">
+        <v>1.0073675799704416</v>
+      </c>
+      <c r="H16">
+        <v>0.20152788034129321</v>
+      </c>
+      <c r="I16">
+        <v>1.1093822909382134</v>
+      </c>
+      <c r="J16">
+        <v>4.5512582667700947</v>
+      </c>
+      <c r="K16">
+        <v>1.368256654092485</v>
+      </c>
+      <c r="L16">
+        <v>1.3735528700213759</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>363</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>97</v>
+      </c>
+      <c r="E17">
+        <v>1.3005207514943307</v>
+      </c>
+      <c r="F17">
+        <v>0.57717561600975353</v>
+      </c>
+      <c r="G17">
+        <v>0.51495723473290655</v>
+      </c>
+      <c r="H17">
+        <v>0.70294841235680294</v>
+      </c>
+      <c r="I17">
+        <v>3.3437517611053242</v>
+      </c>
+      <c r="J17">
+        <v>2.3969777034611215</v>
+      </c>
+      <c r="K17">
+        <v>0.85757748348619256</v>
+      </c>
+      <c r="L17">
+        <v>3.6962059407765415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>364</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>47</v>
+      </c>
+      <c r="D18">
+        <v>96</v>
+      </c>
+      <c r="E18">
+        <v>1.1913040680938578</v>
+      </c>
+      <c r="F18">
+        <v>2.7716383340891482</v>
+      </c>
+      <c r="G18">
+        <v>0.7538047835951196</v>
+      </c>
+      <c r="H18">
+        <v>1.403556102327723</v>
+      </c>
+      <c r="I18">
+        <v>1.8391565877704739</v>
+      </c>
+      <c r="J18">
+        <v>20.928937234936782</v>
+      </c>
+      <c r="K18">
+        <v>1.5462695972254077</v>
+      </c>
+      <c r="L18">
+        <v>14.124018902861566</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>365</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>56</v>
+      </c>
+      <c r="D19">
+        <v>56</v>
+      </c>
+      <c r="E19">
+        <v>1.5545033526657723</v>
+      </c>
+      <c r="F19">
+        <v>0.65172683869370385</v>
+      </c>
+      <c r="G19">
+        <v>0.91246567458713124</v>
+      </c>
+      <c r="H19">
+        <v>1.4886844186338519</v>
+      </c>
+      <c r="I19">
+        <v>1.401831262945133</v>
+      </c>
+      <c r="J19">
+        <v>1.8807626877866159</v>
+      </c>
+      <c r="K19">
+        <v>1.0975487126712118</v>
+      </c>
+      <c r="L19">
+        <v>4.9401772186929556</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>366</v>
+      </c>
+      <c r="B20">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>44</v>
+      </c>
+      <c r="E20">
+        <v>0.60630422594000233</v>
+      </c>
+      <c r="F20">
+        <v>0.43171228213222168</v>
+      </c>
+      <c r="G20">
+        <v>1.205700364307714</v>
+      </c>
+      <c r="H20">
+        <v>0.63072298416271244</v>
+      </c>
+      <c r="I20">
+        <v>1.7782067844432052</v>
+      </c>
+      <c r="J20">
+        <v>3.8687361912133866</v>
+      </c>
+      <c r="K20">
+        <v>1.279901295975298</v>
+      </c>
+      <c r="L20">
+        <v>3.5557750641178112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>367</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>53</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>368</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <v>0.4604422330534409</v>
+      </c>
+      <c r="F22">
+        <v>0.85190082645945298</v>
+      </c>
+      <c r="G22">
+        <v>0.54958806023082474</v>
+      </c>
+      <c r="H22">
+        <v>0.35920842846144702</v>
+      </c>
+      <c r="I22">
+        <v>1.7024224531930556</v>
+      </c>
+      <c r="J22">
+        <v>8.4408666893428457</v>
+      </c>
+      <c r="K22">
+        <v>2.302846022813291</v>
+      </c>
+      <c r="L22">
+        <v>3.529129540601688</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>369</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>44</v>
+      </c>
+      <c r="D23">
+        <v>45</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>370</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <v>36</v>
+      </c>
+      <c r="E24">
+        <v>0.85819742035978264</v>
+      </c>
+      <c r="F24">
+        <v>0.41990320116349744</v>
+      </c>
+      <c r="G24">
+        <v>0.54568242095052566</v>
+      </c>
+      <c r="H24">
+        <v>0.27543556803167857</v>
+      </c>
+      <c r="I24">
+        <v>2.2194957465798026</v>
+      </c>
+      <c r="J24">
+        <v>3.9283850257258806</v>
+      </c>
+      <c r="K24">
+        <v>1.4218127926715429</v>
+      </c>
+      <c r="L24">
+        <v>3.5684760514417797</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>371</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>51</v>
+      </c>
+      <c r="E25">
+        <v>2.6551584726474218</v>
+      </c>
+      <c r="F25">
+        <v>6.8638753977394655</v>
+      </c>
+      <c r="G25">
+        <v>1.4602572997125762</v>
+      </c>
+      <c r="H25">
+        <v>1.6190653086422617</v>
+      </c>
+      <c r="I25">
+        <v>1.4828231252655264</v>
+      </c>
+      <c r="J25">
+        <v>14.428893300860112</v>
+      </c>
+      <c r="K25">
+        <v>2.2096464894585077</v>
+      </c>
+      <c r="L25">
+        <v>4.4427500091740111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>372</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>0.35479333154974074</v>
+      </c>
+      <c r="F26">
+        <v>0.16905200367918505</v>
+      </c>
+      <c r="G26">
+        <v>0.50646304380900187</v>
+      </c>
+      <c r="H26">
+        <v>1.2700356379386999</v>
+      </c>
+      <c r="I26">
+        <v>1.3825130362747016</v>
+      </c>
+      <c r="J26">
+        <v>2.0917628869955038</v>
+      </c>
+      <c r="K26">
+        <v>1.4856614307459495</v>
+      </c>
+      <c r="L26">
+        <v>14.816359710663278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>373</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>57</v>
+      </c>
+      <c r="D27">
+        <v>20</v>
+      </c>
+      <c r="E27">
+        <v>0.53573362631772325</v>
+      </c>
+      <c r="F27">
+        <v>0.86362124035462218</v>
+      </c>
+      <c r="G27">
+        <v>0.60259912731656995</v>
+      </c>
+      <c r="H27">
+        <v>0.47891042959158142</v>
+      </c>
+      <c r="I27">
+        <v>1.1560309016064267</v>
+      </c>
+      <c r="J27">
+        <v>6.8832710711364333</v>
+      </c>
+      <c r="K27">
+        <v>1.5812235380011208</v>
+      </c>
+      <c r="L27">
+        <v>4.872073684333265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>374</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>57</v>
+      </c>
+      <c r="D28">
+        <v>53</v>
+      </c>
+      <c r="E28">
+        <v>0.91950655095208655</v>
+      </c>
+      <c r="F28">
+        <v>0.42653654188248658</v>
+      </c>
+      <c r="G28">
+        <v>1.4070893614829194</v>
+      </c>
+      <c r="H28">
+        <v>0.20765728322133406</v>
+      </c>
+      <c r="I28">
+        <v>0.9753542984126029</v>
+      </c>
+      <c r="J28">
+        <v>3.2710624973837237</v>
+      </c>
+      <c r="K28">
+        <v>1.0523999155643795</v>
+      </c>
+      <c r="L28">
+        <v>1.20801660699668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>375</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>31</v>
+      </c>
+      <c r="D29">
+        <v>57</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>376</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>377</v>
+      </c>
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>51</v>
+      </c>
+      <c r="D31">
+        <v>66</v>
+      </c>
+      <c r="E31">
+        <v>0.60280520304119711</v>
+      </c>
+      <c r="F31">
+        <v>0.30110415115283928</v>
+      </c>
+      <c r="G31">
+        <v>0.6404737566818598</v>
+      </c>
+      <c r="H31">
+        <v>0.84569219383150529</v>
+      </c>
+      <c r="I31">
+        <v>1.9243169976832573</v>
+      </c>
+      <c r="J31">
+        <v>3.6769102869518298</v>
+      </c>
+      <c r="K31">
+        <v>1.4987740872425956</v>
+      </c>
+      <c r="L31">
+        <v>6.1870719457205396</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>378</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>379</v>
+      </c>
+      <c r="B33">
+        <v>19</v>
+      </c>
+      <c r="C33">
+        <v>28</v>
+      </c>
+      <c r="D33">
+        <v>45</v>
+      </c>
+      <c r="E33">
+        <v>0.51138350045185577</v>
+      </c>
+      <c r="F33">
+        <v>1.1820674355951479</v>
+      </c>
+      <c r="G33">
+        <v>0.79065338212646807</v>
+      </c>
+      <c r="H33">
+        <v>1.241111028497714</v>
+      </c>
+      <c r="I33">
+        <v>1.2420602333322279</v>
+      </c>
+      <c r="J33">
+        <v>7.7519363772707361</v>
+      </c>
+      <c r="K33">
+        <v>1.4480957363777389</v>
+      </c>
+      <c r="L33">
+        <v>7.6828717214422131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>380</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>54</v>
+      </c>
+      <c r="D34">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <v>1.2975328394125913</v>
+      </c>
+      <c r="F34">
+        <v>1.9841490886663349</v>
+      </c>
+      <c r="G34">
+        <v>1.0329833305703682</v>
+      </c>
+      <c r="H34">
+        <v>0.18227743145750919</v>
+      </c>
+      <c r="I34">
+        <v>1.537631209543856</v>
+      </c>
+      <c r="J34">
+        <v>12.033810098277517</v>
+      </c>
+      <c r="K34">
+        <v>1.5780290698811934</v>
+      </c>
+      <c r="L34">
+        <v>1.7529105389988671</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>381</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <v>28</v>
+      </c>
+      <c r="D35">
+        <v>68</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>382</v>
+      </c>
+      <c r="B36">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36">
+        <v>35</v>
+      </c>
+      <c r="E36">
+        <v>0.48353515698579497</v>
+      </c>
+      <c r="F36">
+        <v>0.67877839383592753</v>
+      </c>
+      <c r="G36">
+        <v>0.99285770911950755</v>
+      </c>
+      <c r="H36">
+        <v>0.20791199477741956</v>
+      </c>
+      <c r="I36">
+        <v>1.7272464171483282</v>
+      </c>
+      <c r="J36">
+        <v>7.0116570506130849</v>
+      </c>
+      <c r="K36">
+        <v>1.192787663679048</v>
+      </c>
+      <c r="L36">
+        <v>2.1497725233622482</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>383</v>
+      </c>
+      <c r="B37">
+        <v>18</v>
+      </c>
+      <c r="C37">
+        <v>38</v>
+      </c>
+      <c r="D37">
+        <v>52</v>
+      </c>
+      <c r="E37">
+        <v>0.3639379383984872</v>
+      </c>
+      <c r="F37">
+        <v>0.92860036941261048</v>
+      </c>
+      <c r="G37">
+        <v>0.869262353341265</v>
+      </c>
+      <c r="H37">
+        <v>0.97502762624822581</v>
+      </c>
+      <c r="I37">
+        <v>1.5199606838908544</v>
+      </c>
+      <c r="J37">
+        <v>10.0816983610835</v>
+      </c>
+      <c r="K37">
+        <v>1.0038487561919103</v>
+      </c>
+      <c r="L37">
         <v>7.4920642694560105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted plotting and creation of plots plots are now .svg or .pdf depending on compatibility added results of RMET data
</commit_message>
<xml_diff>
--- a/results/current-results.xlsx
+++ b/results/current-results.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Dropbox\Documents\Projects\face-perception\face-perception-ssvep\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1513504\Dropbox\Documents\Projects\face-perception\face-perception-ssvep\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1433,7 +1433,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1786,6 +1786,20 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:432" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4229,13 +4243,13 @@
         <v>3.0809305041706292</v>
       </c>
       <c r="G3">
-        <v>0.74200789623072294</v>
+        <v>0.74200789623072283</v>
       </c>
       <c r="H3">
         <v>1.5673493042825624</v>
       </c>
       <c r="I3">
-        <v>2.4174133283148027</v>
+        <v>2.4174133283148032</v>
       </c>
       <c r="J3">
         <v>27.692890741836688</v>
@@ -4264,10 +4278,10 @@
         <v>1.1840242686318765</v>
       </c>
       <c r="F4">
-        <v>0.25255024323328329</v>
+        <v>0.25255024323328323</v>
       </c>
       <c r="G4">
-        <v>0.82453348409839544</v>
+        <v>0.82453348409839533</v>
       </c>
       <c r="H4">
         <v>0.2142329685050344</v>
@@ -4276,10 +4290,10 @@
         <v>1.2803535960372872</v>
       </c>
       <c r="J4">
-        <v>2.4009822466401571</v>
+        <v>2.4009822466401567</v>
       </c>
       <c r="K4">
-        <v>1.7072537640512697</v>
+        <v>1.7072537640512699</v>
       </c>
       <c r="L4">
         <v>4.1307744489502243</v>
@@ -4315,38 +4329,17 @@
       <c r="A6" t="s">
         <v>352</v>
       </c>
-      <c r="B6">
-        <v>23</v>
-      </c>
-      <c r="C6">
-        <v>35</v>
-      </c>
-      <c r="D6">
-        <v>128</v>
-      </c>
-      <c r="E6">
-        <v>0.61983330392284575</v>
-      </c>
-      <c r="F6">
-        <v>0.97939042375459939</v>
-      </c>
-      <c r="G6">
-        <v>0.93751211452175642</v>
-      </c>
-      <c r="H6">
-        <v>0.29964091682538047</v>
-      </c>
       <c r="I6">
-        <v>1.5662909171947099</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>7.5270974330577261</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>1.2130784013153646</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>1.4607016439452358</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:432" x14ac:dyDescent="0.25">
@@ -4354,25 +4347,37 @@
         <v>353</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="D7">
-        <v>43</v>
+        <v>128</v>
+      </c>
+      <c r="E7">
+        <v>0.61983330392284586</v>
+      </c>
+      <c r="F7">
+        <v>0.97939042375458052</v>
+      </c>
+      <c r="G7">
+        <v>0.93751211452175653</v>
+      </c>
+      <c r="H7">
+        <v>0.29964091682538008</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1.5662909171947088</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>7.5270974330575813</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1.2130784013153655</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1.4607016439452338</v>
       </c>
     </row>
     <row r="8" spans="1:432" x14ac:dyDescent="0.25">
@@ -4380,37 +4385,25 @@
         <v>354</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="D8">
-        <v>55</v>
-      </c>
-      <c r="E8">
-        <v>1.2733902269883504</v>
-      </c>
-      <c r="F8">
-        <v>2.6071053949445213</v>
-      </c>
-      <c r="G8">
-        <v>0.777333921663941</v>
-      </c>
-      <c r="H8">
-        <v>0.73082052307966172</v>
+        <v>43</v>
       </c>
       <c r="I8">
-        <v>1.5895861811605503</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>23.231532600527263</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1.1976820461299551</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>7.0399411621393346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:432" x14ac:dyDescent="0.25">
@@ -4421,34 +4414,34 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D9">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E9">
-        <v>0.43276190596107611</v>
+        <v>1.2733902269883506</v>
       </c>
       <c r="F9">
-        <v>0.40452582535926024</v>
+        <v>2.6071053949445213</v>
       </c>
       <c r="G9">
-        <v>0.35351920981336621</v>
+        <v>0.77733392166394089</v>
       </c>
       <c r="H9">
-        <v>0.40370252279079721</v>
+        <v>0.73082052307966161</v>
       </c>
       <c r="I9">
-        <v>1.4776892896071512</v>
+        <v>1.5895861811605505</v>
       </c>
       <c r="J9">
-        <v>6.1031722490919478</v>
+        <v>23.231532600527263</v>
       </c>
       <c r="K9">
-        <v>1.1214489529106546</v>
+        <v>1.1976820461299549</v>
       </c>
       <c r="L9">
-        <v>3.4219142496295887</v>
+        <v>7.0399411621393329</v>
       </c>
     </row>
     <row r="10" spans="1:432" x14ac:dyDescent="0.25">
@@ -4456,37 +4449,37 @@
         <v>356</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D10">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E10">
-        <v>0.81735307371779209</v>
+        <v>0.43276190596107611</v>
       </c>
       <c r="F10">
-        <v>0.22422687086994453</v>
+        <v>0.40452582535926018</v>
       </c>
       <c r="G10">
-        <v>0.96920468542820948</v>
+        <v>0.35351920981336615</v>
       </c>
       <c r="H10">
-        <v>0.75897476419547738</v>
+        <v>0.40370252279079721</v>
       </c>
       <c r="I10">
-        <v>2.7168174654242372</v>
+        <v>1.4776892896071514</v>
       </c>
       <c r="J10">
-        <v>3.8573756561747201</v>
+        <v>6.1031722490919469</v>
       </c>
       <c r="K10">
-        <v>2.9085648918613867</v>
+        <v>1.1214489529106544</v>
       </c>
       <c r="L10">
-        <v>11.416108005551136</v>
+        <v>3.4219142496295896</v>
       </c>
     </row>
     <row r="11" spans="1:432" x14ac:dyDescent="0.25">
@@ -4494,37 +4487,37 @@
         <v>357</v>
       </c>
       <c r="B11">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D11">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E11">
-        <v>1.4381902729625031</v>
+        <v>0.81735307371779209</v>
       </c>
       <c r="F11">
-        <v>3.7478913396772224</v>
+        <v>0.22422687086994456</v>
       </c>
       <c r="G11">
-        <v>0.81537868174936956</v>
+        <v>0.96920468542820948</v>
       </c>
       <c r="H11">
-        <v>0.30898335539981941</v>
+        <v>0.75897476419547738</v>
       </c>
       <c r="I11">
-        <v>1.4114017973177295</v>
+        <v>2.7168174654242372</v>
       </c>
       <c r="J11">
-        <v>14.296792908110298</v>
+        <v>3.8573756561747206</v>
       </c>
       <c r="K11">
-        <v>1.1257482063992477</v>
+        <v>2.9085648918613862</v>
       </c>
       <c r="L11">
-        <v>1.757365072500835</v>
+        <v>11.416108005551136</v>
       </c>
     </row>
     <row r="12" spans="1:432" x14ac:dyDescent="0.25">
@@ -4532,37 +4525,37 @@
         <v>358</v>
       </c>
       <c r="B12">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D12">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E12">
-        <v>0.95379519673090774</v>
+        <v>1.4381902729625036</v>
       </c>
       <c r="F12">
-        <v>0.36097002433204217</v>
+        <v>3.7478913396772224</v>
       </c>
       <c r="G12">
-        <v>0.42108852151425868</v>
+        <v>0.81537868174936956</v>
       </c>
       <c r="H12">
-        <v>0.47767260513355725</v>
+        <v>0.30898335539981947</v>
       </c>
       <c r="I12">
-        <v>2.4585801332953232</v>
+        <v>1.4114017973177297</v>
       </c>
       <c r="J12">
-        <v>5.3702019630686681</v>
+        <v>14.296792908110298</v>
       </c>
       <c r="K12">
-        <v>1.1136558533705563</v>
+        <v>1.1257482063992477</v>
       </c>
       <c r="L12">
-        <v>7.1549162374821611</v>
+        <v>1.7573650725008343</v>
       </c>
     </row>
     <row r="13" spans="1:432" x14ac:dyDescent="0.25">
@@ -4570,25 +4563,37 @@
         <v>359</v>
       </c>
       <c r="B13">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D13">
-        <v>34</v>
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>0.95379519673090785</v>
+      </c>
+      <c r="F13">
+        <v>0.36097002433204217</v>
+      </c>
+      <c r="G13">
+        <v>0.4210885215142588</v>
+      </c>
+      <c r="H13">
+        <v>0.47767260513355747</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>2.4585801332953228</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>5.3702019630686708</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1.1136558533705563</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>7.1549162374821673</v>
       </c>
     </row>
     <row r="14" spans="1:432" x14ac:dyDescent="0.25">
@@ -4596,13 +4601,13 @@
         <v>360</v>
       </c>
       <c r="B14">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D14">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -4622,37 +4627,25 @@
         <v>361</v>
       </c>
       <c r="B15">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D15">
-        <v>68</v>
-      </c>
-      <c r="E15">
-        <v>0.47468458312320949</v>
-      </c>
-      <c r="F15">
-        <v>0.8777857084531443</v>
-      </c>
-      <c r="G15">
-        <v>0.34492644847508674</v>
-      </c>
-      <c r="H15">
-        <v>0.77281239479623187</v>
+        <v>65</v>
       </c>
       <c r="I15">
-        <v>1.4197699583819678</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>8.9529103944407424</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1.2309623848790963</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>8.5736497901524338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:432" x14ac:dyDescent="0.25">
@@ -4660,37 +4653,37 @@
         <v>362</v>
       </c>
       <c r="B16">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D16">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E16">
-        <v>1.0565796163817847</v>
+        <v>0.47468458312320949</v>
       </c>
       <c r="F16">
-        <v>1.4604124494786559</v>
+        <v>0.87778570845314496</v>
       </c>
       <c r="G16">
-        <v>1.1197483558662329</v>
+        <v>0.34492644847508674</v>
       </c>
       <c r="H16">
-        <v>0.21414542919904742</v>
+        <v>0.77281239479623176</v>
       </c>
       <c r="I16">
-        <v>1.1017068495166564</v>
+        <v>1.4197699583819678</v>
       </c>
       <c r="J16">
-        <v>8.5931380090230451</v>
+        <v>8.9529103944407442</v>
       </c>
       <c r="K16">
-        <v>1.5514842060938723</v>
+        <v>1.2309623848790963</v>
       </c>
       <c r="L16">
-        <v>1.8539866536097023</v>
+        <v>8.5736497901524302</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -4698,37 +4691,37 @@
         <v>363</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="E17">
-        <v>1.1081014179609243</v>
+        <v>1.0565796163817847</v>
       </c>
       <c r="F17">
-        <v>0.83870128504007235</v>
+        <v>1.4604124494786559</v>
       </c>
       <c r="G17">
-        <v>0.55414629919432012</v>
+        <v>1.1197483558662331</v>
       </c>
       <c r="H17">
-        <v>1.138926002509858</v>
+        <v>0.21414542919904739</v>
       </c>
       <c r="I17">
-        <v>3.0498365941733456</v>
+        <v>1.1017068495166562</v>
       </c>
       <c r="J17">
-        <v>3.8183491459507968</v>
+        <v>8.5931380090230451</v>
       </c>
       <c r="K17">
-        <v>0.9339821603987164</v>
+        <v>1.5514842060938723</v>
       </c>
       <c r="L17">
-        <v>6.3056748961770026</v>
+        <v>1.8539866536097023</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -4739,34 +4732,34 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D18">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E18">
-        <v>1.2735983646056854</v>
+        <v>1.1081014179609243</v>
       </c>
       <c r="F18">
-        <v>4.7891582649633353</v>
+        <v>0.83870128504007269</v>
       </c>
       <c r="G18">
-        <v>0.84708859132750902</v>
+        <v>0.55414629919432001</v>
       </c>
       <c r="H18">
-        <v>2.3676897835772666</v>
+        <v>1.1389260025098575</v>
       </c>
       <c r="I18">
-        <v>1.7622450788221391</v>
+        <v>3.0498365941733461</v>
       </c>
       <c r="J18">
-        <v>40.04866606233179</v>
+        <v>3.818349145950799</v>
       </c>
       <c r="K18">
-        <v>1.6623622689052155</v>
+        <v>0.9339821603987164</v>
       </c>
       <c r="L18">
-        <v>26.304964702085346</v>
+        <v>6.3056748961770008</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -4774,37 +4767,37 @@
         <v>365</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D19">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="E19">
-        <v>1.2340705010419366</v>
+        <v>1.2735983646056854</v>
       </c>
       <c r="F19">
-        <v>0.76989769332056168</v>
+        <v>4.7891582649633353</v>
       </c>
       <c r="G19">
-        <v>0.64333451355617721</v>
+        <v>0.84708859132750924</v>
       </c>
       <c r="H19">
-        <v>2.2407290038351504</v>
+        <v>2.3676897835772666</v>
       </c>
       <c r="I19">
-        <v>1.4040705144642072</v>
+        <v>1.7622450788221391</v>
       </c>
       <c r="J19">
-        <v>2.6994980781516098</v>
+        <v>40.048666062331776</v>
       </c>
       <c r="K19">
-        <v>1.0110937680035335</v>
+        <v>1.6623622689052155</v>
       </c>
       <c r="L19">
-        <v>8.7371119274152242</v>
+        <v>26.304964702085353</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -4812,37 +4805,37 @@
         <v>366</v>
       </c>
       <c r="B20">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D20">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E20">
-        <v>0.73600764976239941</v>
+        <v>1.2340705010419366</v>
       </c>
       <c r="F20">
-        <v>0.60711403222426752</v>
+        <v>0.76989769332056168</v>
       </c>
       <c r="G20">
-        <v>1.1543907853447979</v>
+        <v>0.64333451355617732</v>
       </c>
       <c r="H20">
-        <v>0.93289576399489171</v>
+        <v>2.2407290038351499</v>
       </c>
       <c r="I20">
-        <v>1.7634365031264263</v>
+        <v>1.4040705144642072</v>
       </c>
       <c r="J20">
-        <v>6.0888374793708975</v>
+        <v>2.6994980781516098</v>
       </c>
       <c r="K20">
-        <v>1.2494963107863799</v>
+        <v>1.0110937680035335</v>
       </c>
       <c r="L20">
-        <v>5.9112810120140056</v>
+        <v>8.7371119274152225</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -4850,37 +4843,37 @@
         <v>367</v>
       </c>
       <c r="B21">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E21">
-        <v>0.89920904561645143</v>
+        <v>0.73600764976239941</v>
       </c>
       <c r="F21">
-        <v>0.41136795032389739</v>
+        <v>0.60711403222426752</v>
       </c>
       <c r="G21">
-        <v>0.73991983527403782</v>
+        <v>1.1543907853447983</v>
       </c>
       <c r="H21">
-        <v>0.20021670267537978</v>
+        <v>0.93289576399489171</v>
       </c>
       <c r="I21">
-        <v>1.1385198959113014</v>
+        <v>1.7634365031264263</v>
       </c>
       <c r="J21">
-        <v>3.2090623495619606</v>
+        <v>6.0888374793708975</v>
       </c>
       <c r="K21">
-        <v>1.11543307493987</v>
+        <v>1.2494963107863797</v>
       </c>
       <c r="L21">
-        <v>2.8317360695868303</v>
+        <v>5.9112810120140056</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -4888,37 +4881,37 @@
         <v>368</v>
       </c>
       <c r="B22">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D22">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E22">
-        <v>0.44694514061718943</v>
+        <v>0.89920904561645143</v>
       </c>
       <c r="F22">
-        <v>1.4041372314057812</v>
+        <v>0.41136795032389739</v>
       </c>
       <c r="G22">
-        <v>0.49440575468138059</v>
+        <v>0.73991983527403793</v>
       </c>
       <c r="H22">
-        <v>0.53082283159668642</v>
+        <v>0.20021670267537978</v>
       </c>
       <c r="I22">
-        <v>1.8539716306704068</v>
+        <v>1.1385198959113012</v>
       </c>
       <c r="J22">
-        <v>14.370630998100447</v>
+        <v>3.2090623495619619</v>
       </c>
       <c r="K22">
-        <v>2.1818290377257772</v>
+        <v>1.1154330749398704</v>
       </c>
       <c r="L22">
-        <v>5.9278410225989679</v>
+        <v>2.8317360695868299</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -4926,37 +4919,37 @@
         <v>369</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C23">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D23">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E23">
-        <v>0.84039411144137122</v>
+        <v>0.44694514061718948</v>
       </c>
       <c r="F23">
-        <v>0.40247152051518365</v>
+        <v>1.4041372314057812</v>
       </c>
       <c r="G23">
-        <v>0.59245004196028628</v>
+        <v>0.49440575468138059</v>
       </c>
       <c r="H23">
-        <v>0.17414674232212241</v>
+        <v>0.53082283159668631</v>
       </c>
       <c r="I23">
-        <v>0.78984431612191697</v>
+        <v>1.853971630670407</v>
       </c>
       <c r="J23">
-        <v>2.3759839865629657</v>
+        <v>14.370630998100447</v>
       </c>
       <c r="K23">
-        <v>1.0727457505424669</v>
+        <v>2.1818290377257772</v>
       </c>
       <c r="L23">
-        <v>1.4141187560515063</v>
+        <v>5.9278410225989671</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -4964,37 +4957,37 @@
         <v>370</v>
       </c>
       <c r="B24">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D24">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E24">
-        <v>1.216776541485183</v>
+        <v>0.84039411144137099</v>
       </c>
       <c r="F24">
-        <v>0.69555904874422514</v>
+        <v>0.40247152051518359</v>
       </c>
       <c r="G24">
-        <v>0.59873616662213214</v>
+        <v>0.59245004196028639</v>
       </c>
       <c r="H24">
-        <v>0.39253040033564973</v>
+        <v>0.17414674232212241</v>
       </c>
       <c r="I24">
-        <v>2.4406737148481823</v>
+        <v>0.78984431612191663</v>
       </c>
       <c r="J24">
-        <v>7.6120296778434682</v>
+        <v>2.3759839865629657</v>
       </c>
       <c r="K24">
-        <v>1.3580278676789261</v>
+        <v>1.0727457505424667</v>
       </c>
       <c r="L24">
-        <v>5.7873504593576834</v>
+        <v>1.4141187560515063</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -5002,37 +4995,37 @@
         <v>371</v>
       </c>
       <c r="B25">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C25">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D25">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E25">
-        <v>3.2257947096990769</v>
+        <v>1.216776541485183</v>
       </c>
       <c r="F25">
-        <v>12.148070841272705</v>
+        <v>0.69555904874422514</v>
       </c>
       <c r="G25">
-        <v>1.5777963193154076</v>
+        <v>0.59873616662213203</v>
       </c>
       <c r="H25">
-        <v>2.4245919322483589</v>
+        <v>0.39253040033564979</v>
       </c>
       <c r="I25">
-        <v>1.5142226500158731</v>
+        <v>2.4406737148481823</v>
       </c>
       <c r="J25">
-        <v>28.583469473898926</v>
+        <v>7.6120296778434682</v>
       </c>
       <c r="K25">
-        <v>2.1925786470200666</v>
+        <v>1.3580278676789259</v>
       </c>
       <c r="L25">
-        <v>7.4558172273652845</v>
+        <v>5.7873504593576843</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -5040,37 +5033,37 @@
         <v>372</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C26">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D26">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E26">
-        <v>0.28842347369795918</v>
+        <v>3.2257947096990769</v>
       </c>
       <c r="F26">
-        <v>0.27742495755089885</v>
+        <v>12.148070841272705</v>
       </c>
       <c r="G26">
-        <v>0.42252544418754912</v>
+        <v>1.5777963193154076</v>
       </c>
       <c r="H26">
-        <v>2.243015441445364</v>
+        <v>2.4245919322483593</v>
       </c>
       <c r="I26">
-        <v>1.3287006855076822</v>
+        <v>1.5142226500158726</v>
       </c>
       <c r="J26">
-        <v>3.7782494820101298</v>
+        <v>28.583469473898919</v>
       </c>
       <c r="K26">
-        <v>1.4078037971373003</v>
+        <v>2.192578647020067</v>
       </c>
       <c r="L26">
-        <v>30.178226579148962</v>
+        <v>7.4558172273652827</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -5078,37 +5071,37 @@
         <v>373</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D27">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E27">
-        <v>0.50789904727706969</v>
+        <v>0.28842347369795918</v>
       </c>
       <c r="F27">
-        <v>1.3947151891994345</v>
+        <v>0.27742495755089885</v>
       </c>
       <c r="G27">
-        <v>0.53759826539938649</v>
+        <v>0.42252544418754912</v>
       </c>
       <c r="H27">
-        <v>0.65398665211188267</v>
+        <v>2.243015441445364</v>
       </c>
       <c r="I27">
-        <v>1.1003865551196736</v>
+        <v>1.3287006855076822</v>
       </c>
       <c r="J27">
-        <v>13.257813387330623</v>
+        <v>3.7782494820101298</v>
       </c>
       <c r="K27">
-        <v>1.5225378860526293</v>
+        <v>1.4078037971373003</v>
       </c>
       <c r="L27">
-        <v>7.5188042337657812</v>
+        <v>30.178226579148962</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -5116,37 +5109,37 @@
         <v>374</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>57</v>
       </c>
       <c r="D28">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="E28">
-        <v>0.89162148211253445</v>
+        <v>0.50789904727706969</v>
       </c>
       <c r="F28">
-        <v>0.66663898612285566</v>
+        <v>1.3947151891994345</v>
       </c>
       <c r="G28">
-        <v>1.2745737554046543</v>
+        <v>0.53759826539938649</v>
       </c>
       <c r="H28">
-        <v>0.16711351072259795</v>
+        <v>0.65398665211188278</v>
       </c>
       <c r="I28">
-        <v>0.96219236811588094</v>
+        <v>1.1003865551196736</v>
       </c>
       <c r="J28">
-        <v>5.825286577858213</v>
+        <v>13.257813387330623</v>
       </c>
       <c r="K28">
-        <v>0.87311326106674647</v>
+        <v>1.5225378860526293</v>
       </c>
       <c r="L28">
-        <v>1.0725648890418609</v>
+        <v>7.518804233765783</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -5154,31 +5147,52 @@
         <v>375</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="D29">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="E29">
+        <v>0.89162148211253456</v>
+      </c>
+      <c r="F29">
+        <v>0.66663898612285577</v>
+      </c>
+      <c r="G29">
+        <v>1.2745737554046543</v>
+      </c>
+      <c r="H29">
+        <v>0.16711351072259789</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>0.96219236811588083</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>5.8252865778582255</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>0.87311326106674647</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>1.0725648890418604</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>376</v>
       </c>
+      <c r="B30">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>31</v>
+      </c>
+      <c r="D30">
+        <v>57</v>
+      </c>
       <c r="I30">
         <v>0</v>
       </c>
@@ -5209,25 +5223,25 @@
         <v>0.51316010179114091</v>
       </c>
       <c r="F31">
-        <v>0.4986433472436459</v>
+        <v>0.49864334724364651</v>
       </c>
       <c r="G31">
-        <v>0.53944051662119297</v>
+        <v>0.53944051662119286</v>
       </c>
       <c r="H31">
-        <v>1.3738008298734443</v>
+        <v>1.3738008298734454</v>
       </c>
       <c r="I31">
         <v>1.7300683208124952</v>
       </c>
       <c r="J31">
-        <v>6.8182112111284816</v>
+        <v>6.8182112111284914</v>
       </c>
       <c r="K31">
-        <v>1.3601468507923631</v>
+        <v>1.3601468507923637</v>
       </c>
       <c r="L31">
-        <v>12.279126781974561</v>
+        <v>12.279126781974572</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -5264,25 +5278,25 @@
         <v>0.52035876274418835</v>
       </c>
       <c r="F33">
-        <v>1.9938608303487835</v>
+        <v>1.993860830348783</v>
       </c>
       <c r="G33">
-        <v>0.69565020747540784</v>
+        <v>0.69565020747540807</v>
       </c>
       <c r="H33">
-        <v>2.1169293066713109</v>
+        <v>2.1169293066713113</v>
       </c>
       <c r="I33">
         <v>1.3973245318916649</v>
       </c>
       <c r="J33">
-        <v>14.566179196773849</v>
+        <v>14.566179196773842</v>
       </c>
       <c r="K33">
-        <v>1.4716114283756776</v>
+        <v>1.4716114283756774</v>
       </c>
       <c r="L33">
-        <v>14.228141992656763</v>
+        <v>14.228141992656765</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -5302,7 +5316,7 @@
         <v>1.3265022450711097</v>
       </c>
       <c r="F34">
-        <v>3.4300463563059429</v>
+        <v>3.4300463563059433</v>
       </c>
       <c r="G34">
         <v>1.1260083885570085</v>
@@ -5314,7 +5328,7 @@
         <v>1.6625692937608914</v>
       </c>
       <c r="J34">
-        <v>22.942954738814386</v>
+        <v>22.94295473881439</v>
       </c>
       <c r="K34">
         <v>1.6309341251908067</v>
@@ -5363,28 +5377,28 @@
         <v>35</v>
       </c>
       <c r="E36">
-        <v>0.40639558059665515</v>
+        <v>0.4063955805966552</v>
       </c>
       <c r="F36">
-        <v>1.1469214893116977</v>
+        <v>1.1469214893116981</v>
       </c>
       <c r="G36">
-        <v>1.1535438803244873</v>
+        <v>1.1535438803244877</v>
       </c>
       <c r="H36">
-        <v>0.33029228455908499</v>
+        <v>0.33029228455908466</v>
       </c>
       <c r="I36">
-        <v>1.5055924200132249</v>
+        <v>1.5055924200132254</v>
       </c>
       <c r="J36">
-        <v>13.559559229966498</v>
+        <v>13.559559229966503</v>
       </c>
       <c r="K36">
-        <v>1.172005245153217</v>
+        <v>1.1720052451532166</v>
       </c>
       <c r="L36">
-        <v>4.1662961176431539</v>
+        <v>4.1662961176431503</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -5401,28 +5415,28 @@
         <v>52</v>
       </c>
       <c r="E37">
-        <v>0.32455097257726068</v>
+        <v>0.32455097257726073</v>
       </c>
       <c r="F37">
-        <v>1.5419524991894278</v>
+        <v>1.5419524991894284</v>
       </c>
       <c r="G37">
         <v>0.77389897895853965</v>
       </c>
       <c r="H37">
-        <v>1.7658376297430309</v>
+        <v>1.7658376297430305</v>
       </c>
       <c r="I37">
         <v>1.5187067591647232</v>
       </c>
       <c r="J37">
-        <v>19.775872112522574</v>
+        <v>19.775872112522581</v>
       </c>
       <c r="K37">
-        <v>1.0052427211092048</v>
+        <v>1.0052427211092045</v>
       </c>
       <c r="L37">
-        <v>15.85637088776533</v>
+        <v>15.856370887765326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>